<commit_message>
avg price & posts plot changed to plotly
</commit_message>
<xml_diff>
--- a/Lithuania coronavirus data.xlsx
+++ b/Lithuania coronavirus data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tiesi\Class D\Vilnius-Real-Estate-market-exploration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E59E829C-755A-4D3D-9830-8F0F39AF626F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBBC12A6-A83C-4C86-B101-A862B20BC48F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25710" yWindow="8500" windowWidth="28800" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="structured" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="118">
   <si>
     <r>
       <t>December 2019:</t>
@@ -4770,6 +4770,12 @@
       </rPr>
       <t>[99]</t>
     </r>
+  </si>
+  <si>
+    <t>week 15</t>
+  </si>
+  <si>
+    <t>week 25</t>
   </si>
 </sst>
 </file>
@@ -5177,20 +5183,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1034DBB8-50E9-45D8-A6FB-1177C8125CE6}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:C58"/>
+  <dimension ref="A1:D58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.54296875" customWidth="1"/>
-    <col min="2" max="2" width="70.26953125" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" customWidth="1"/>
+    <col min="2" max="2" width="70.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>102</v>
       </c>
@@ -5201,7 +5206,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>43800</v>
       </c>
@@ -5212,7 +5217,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>43855</v>
       </c>
@@ -5223,7 +5228,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>43887</v>
       </c>
@@ -5234,7 +5239,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>43889</v>
       </c>
@@ -5245,7 +5250,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="6" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>43900</v>
       </c>
@@ -5256,7 +5261,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>43902</v>
       </c>
@@ -5267,7 +5272,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="8" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>43903</v>
       </c>
@@ -5278,7 +5283,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>43904</v>
       </c>
@@ -5289,7 +5294,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>43905</v>
       </c>
@@ -5300,7 +5305,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>43906</v>
       </c>
@@ -5311,7 +5316,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" ht="144" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>43907</v>
       </c>
@@ -5322,7 +5327,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>43908</v>
       </c>
@@ -5333,7 +5338,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" ht="144" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>43909</v>
       </c>
@@ -5344,7 +5349,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>43910</v>
       </c>
@@ -5355,7 +5360,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="16" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>43911</v>
       </c>
@@ -5366,7 +5371,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="17" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>43912</v>
       </c>
@@ -5377,7 +5382,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="18" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>43913</v>
       </c>
@@ -5388,7 +5393,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>43914</v>
       </c>
@@ -5399,7 +5404,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>43915</v>
       </c>
@@ -5410,7 +5415,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="21" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>43917</v>
       </c>
@@ -5421,7 +5426,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="22" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>43918</v>
       </c>
@@ -5432,7 +5437,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <v>43920</v>
       </c>
@@ -5443,7 +5448,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="24" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>43921</v>
       </c>
@@ -5454,7 +5459,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
         <v>43922</v>
       </c>
@@ -5465,7 +5470,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
         <v>43923</v>
       </c>
@@ -5476,7 +5481,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="4">
         <v>43924</v>
       </c>
@@ -5487,7 +5492,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A28" s="4">
         <v>43925</v>
       </c>
@@ -5498,7 +5503,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A29" s="4">
         <v>43926</v>
       </c>
@@ -5509,7 +5514,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="30" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A30" s="4">
         <v>43927</v>
       </c>
@@ -5520,7 +5525,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="31" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="4">
         <v>43928</v>
       </c>
@@ -5531,7 +5536,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
         <v>43929</v>
       </c>
@@ -5541,8 +5546,11 @@
       <c r="C32" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
+      <c r="D32" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
         <v>43930</v>
       </c>
@@ -5553,7 +5561,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
         <v>43931</v>
       </c>
@@ -5564,7 +5572,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="35" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="4">
         <v>43932</v>
       </c>
@@ -5575,7 +5583,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A36" s="4">
         <v>43935</v>
       </c>
@@ -5586,7 +5594,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="159.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
         <v>43936</v>
       </c>
@@ -5597,7 +5605,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A38" s="4">
         <v>43939</v>
       </c>
@@ -5608,7 +5616,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A39" s="4">
         <v>43943</v>
       </c>
@@ -5619,7 +5627,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" s="4">
         <v>43944</v>
       </c>
@@ -5630,7 +5638,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="116" hidden="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A41" s="4">
         <v>43948</v>
       </c>
@@ -5638,7 +5646,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="116" hidden="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A42" s="4">
         <v>43950</v>
       </c>
@@ -5649,7 +5657,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A43" s="4">
         <v>43955</v>
       </c>
@@ -5660,7 +5668,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A44" s="4">
         <v>43957</v>
       </c>
@@ -5671,7 +5679,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="188.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A45" s="4">
         <v>43962</v>
       </c>
@@ -5682,7 +5690,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="87" hidden="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A46" s="4">
         <v>43964</v>
       </c>
@@ -5693,7 +5701,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A47" s="4">
         <v>43965</v>
       </c>
@@ -5704,7 +5712,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A48" s="4">
         <v>43966</v>
       </c>
@@ -5715,7 +5723,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A49" s="4">
         <v>43969</v>
       </c>
@@ -5726,7 +5734,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A50" s="4">
         <v>43976</v>
       </c>
@@ -5737,7 +5745,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A51" s="4">
         <v>43978</v>
       </c>
@@ -5748,7 +5756,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A52" s="4">
         <v>43981</v>
       </c>
@@ -5759,7 +5767,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A53" s="4">
         <v>43983</v>
       </c>
@@ -5770,7 +5778,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="54" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="4">
         <v>43992</v>
       </c>
@@ -5781,18 +5789,21 @@
         <v>111</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="4">
         <v>43999</v>
       </c>
-      <c r="B55" s="5" t="s">
+      <c r="B55" s="6" t="s">
         <v>100</v>
       </c>
       <c r="C55" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
+      <c r="D55" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A56" s="4">
         <v>44027</v>
       </c>
@@ -5803,17 +5814,11 @@
         <v>111</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C56" xr:uid="{7C29C219-7012-4E07-9AD0-E1E3AEC43F1D}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="Major"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:C56" xr:uid="{7C29C219-7012-4E07-9AD0-E1E3AEC43F1D}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -5827,287 +5832,287 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="203.7265625" customWidth="1"/>
+    <col min="1" max="1" width="203.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1" ht="19.2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1" ht="19.2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1" ht="19.2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="27" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="27" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:1" ht="19.2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="27" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:1" ht="19.2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="36" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" ht="38.4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" ht="19.2" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1" ht="19.2" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:1" ht="19.2" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1" ht="27" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:1" ht="19.2" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:1" ht="27" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:1" ht="38.4" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:1" ht="19.2" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="1:1" ht="21" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="3"/>
     </row>
   </sheetData>

</xml_diff>